<commit_message>
change the imaclim aggreg
</commit_message>
<xml_diff>
--- a/data/aggregation/IMACLIM_format.xlsx
+++ b/data/aggregation/IMACLIM_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mpotfer\Stage\MatMat-Trade\data\aggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEB8E7D-7BE0-40F9-81B2-FB7DF49EA5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891722F4-BA1E-4498-9C4B-D2EDEEF2A3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sectors" sheetId="1" r:id="rId1"/>
@@ -1589,9 +1589,9 @@
   </sheetPr>
   <dimension ref="A1:T202"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E198" sqref="E198"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5377,13 +5377,13 @@
         <v>0</v>
       </c>
       <c r="K73" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L73" s="16">
         <v>0</v>
       </c>
       <c r="M73" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N73" s="16">
         <v>0</v>
@@ -5429,13 +5429,13 @@
         <v>0</v>
       </c>
       <c r="K74" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74" s="16">
         <v>0</v>
       </c>
       <c r="M74" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N74" s="16">
         <v>0</v>
@@ -12074,8 +12074,8 @@
   </sheetPr>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add the names of sectors to aggreg matrix
</commit_message>
<xml_diff>
--- a/data/aggregation/IMACLIM_format.xlsx
+++ b/data/aggregation/IMACLIM_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mpotfer\Stage\MatMat-Trade\data\aggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1072EF97-8E45-4C82-90BF-5C189BF875A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AF7129-0045-4395-86E2-399F4E63BD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sectors" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="365">
   <si>
     <t>Country name</t>
   </si>
@@ -1069,6 +1069,66 @@
   </si>
   <si>
     <t>Extra-territorial organizations and bodies</t>
+  </si>
+  <si>
+    <t>Nuclear_fuel</t>
+  </si>
+  <si>
+    <t>Bioenergy</t>
+  </si>
+  <si>
+    <t>Transport_equipment</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Energy_Services</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
+    <t>Water_and_waste_treatment</t>
+  </si>
+  <si>
+    <t>Water_services</t>
+  </si>
+  <si>
+    <t>Oth_services</t>
+  </si>
+  <si>
+    <t>Business_services</t>
+  </si>
+  <si>
+    <t>Trade_services</t>
+  </si>
+  <si>
+    <t>Transports</t>
+  </si>
+  <si>
+    <t>Land_transport</t>
+  </si>
+  <si>
+    <t>Water_transport</t>
+  </si>
+  <si>
+    <t>Air_transport</t>
+  </si>
+  <si>
+    <t>Public_services</t>
+  </si>
+  <si>
+    <t>Incineration</t>
+  </si>
+  <si>
+    <t>Land_application</t>
+  </si>
+  <si>
+    <t>Other_waste_treatment</t>
+  </si>
+  <si>
+    <t>Landfill</t>
   </si>
 </sst>
 </file>
@@ -1286,7 +1346,68 @@
     <cellStyle name="Normal 3" xfId="2" xr:uid="{D5EF13C6-0C57-4995-BABD-C212ED929AD5}"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{726504C3-CF01-41A5-A799-31D8A7D4A0C4}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1590,13 +1711,14 @@
   <dimension ref="A1:T202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K93" sqref="K93"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" style="3" customWidth="1"/>
     <col min="4" max="14" width="11.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.6640625" style="3" customWidth="1"/>
@@ -1656,7 +1778,9 @@
       <c r="T1" s="4"/>
     </row>
     <row r="2" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
+      <c r="A2" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="B2" s="6" t="s">
         <v>105</v>
       </c>
@@ -5762,11 +5886,11 @@
       <c r="T80" s="9"/>
     </row>
     <row r="81" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="8">
-        <v>0</v>
-      </c>
-      <c r="B81" s="9">
-        <v>0</v>
+      <c r="A81" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="C81" t="s">
         <v>224</v>
@@ -5814,11 +5938,11 @@
       <c r="T81" s="9"/>
     </row>
     <row r="82" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="8">
-        <v>0</v>
-      </c>
-      <c r="B82" s="9">
-        <v>0</v>
+      <c r="A82" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="C82" t="s">
         <v>225</v>
@@ -5866,11 +5990,11 @@
       <c r="T82" s="9"/>
     </row>
     <row r="83" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="8">
-        <v>0</v>
-      </c>
-      <c r="B83" s="9">
-        <v>0</v>
+      <c r="A83" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="C83" t="s">
         <v>226</v>
@@ -5918,11 +6042,11 @@
       <c r="T83" s="9"/>
     </row>
     <row r="84" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="8">
-        <v>0</v>
-      </c>
-      <c r="B84" s="9">
-        <v>0</v>
+      <c r="A84" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="C84" t="s">
         <v>227</v>
@@ -5970,11 +6094,11 @@
       <c r="T84" s="9"/>
     </row>
     <row r="85" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="8">
-        <v>0</v>
-      </c>
-      <c r="B85" s="9">
-        <v>0</v>
+      <c r="A85" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="C85" t="s">
         <v>228</v>
@@ -6022,11 +6146,11 @@
       <c r="T85" s="9"/>
     </row>
     <row r="86" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="8">
-        <v>0</v>
-      </c>
-      <c r="B86" s="9">
-        <v>0</v>
+      <c r="A86" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>345</v>
       </c>
       <c r="C86" t="s">
         <v>229</v>
@@ -6074,11 +6198,11 @@
       <c r="T86" s="9"/>
     </row>
     <row r="87" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="8">
-        <v>0</v>
-      </c>
-      <c r="B87" s="9">
-        <v>0</v>
+      <c r="A87" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C87" t="s">
         <v>230</v>
@@ -6126,11 +6250,11 @@
       <c r="T87" s="9"/>
     </row>
     <row r="88" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="8">
-        <v>0</v>
-      </c>
-      <c r="B88" s="9">
-        <v>0</v>
+      <c r="A88" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C88" t="s">
         <v>231</v>
@@ -6178,11 +6302,11 @@
       <c r="T88" s="9"/>
     </row>
     <row r="89" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="8">
-        <v>0</v>
-      </c>
-      <c r="B89" s="9">
-        <v>0</v>
+      <c r="A89" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C89" t="s">
         <v>232</v>
@@ -6230,11 +6354,11 @@
       <c r="T89" s="9"/>
     </row>
     <row r="90" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="8">
-        <v>0</v>
-      </c>
-      <c r="B90" s="9">
-        <v>0</v>
+      <c r="A90" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C90" t="s">
         <v>233</v>
@@ -6282,11 +6406,11 @@
       <c r="T90" s="9"/>
     </row>
     <row r="91" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="8">
-        <v>0</v>
-      </c>
-      <c r="B91" s="9">
-        <v>0</v>
+      <c r="A91" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C91" t="s">
         <v>234</v>
@@ -6334,11 +6458,11 @@
       <c r="T91" s="9"/>
     </row>
     <row r="92" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="8">
-        <v>0</v>
-      </c>
-      <c r="B92" s="9">
-        <v>0</v>
+      <c r="A92" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>346</v>
       </c>
       <c r="C92" t="s">
         <v>235</v>
@@ -6386,11 +6510,11 @@
       <c r="T92" s="9"/>
     </row>
     <row r="93" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="8">
-        <v>0</v>
-      </c>
-      <c r="B93" s="9">
-        <v>0</v>
+      <c r="A93" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="C93" t="s">
         <v>236</v>
@@ -6438,11 +6562,11 @@
       <c r="T93" s="9"/>
     </row>
     <row r="94" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="8">
-        <v>0</v>
-      </c>
-      <c r="B94" s="9">
-        <v>0</v>
+      <c r="A94" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>346</v>
       </c>
       <c r="C94" t="s">
         <v>237</v>
@@ -6490,11 +6614,11 @@
       <c r="T94" s="9"/>
     </row>
     <row r="95" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="8">
-        <v>0</v>
-      </c>
-      <c r="B95" s="9">
-        <v>0</v>
+      <c r="A95" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>346</v>
       </c>
       <c r="C95" t="s">
         <v>238</v>
@@ -6542,11 +6666,11 @@
       <c r="T95" s="9"/>
     </row>
     <row r="96" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="8">
-        <v>0</v>
-      </c>
-      <c r="B96" s="9">
-        <v>0</v>
+      <c r="A96" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>346</v>
       </c>
       <c r="C96" t="s">
         <v>239</v>
@@ -6594,11 +6718,11 @@
       <c r="T96" s="9"/>
     </row>
     <row r="97" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="8">
-        <v>0</v>
-      </c>
-      <c r="B97" s="9">
-        <v>0</v>
+      <c r="A97" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="C97" t="s">
         <v>240</v>
@@ -6646,11 +6770,11 @@
       <c r="T97" s="9"/>
     </row>
     <row r="98" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="8">
-        <v>0</v>
-      </c>
-      <c r="B98" s="9">
-        <v>0</v>
+      <c r="A98" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C98" t="s">
         <v>241</v>
@@ -6698,11 +6822,11 @@
       <c r="T98" s="9"/>
     </row>
     <row r="99" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="8">
-        <v>0</v>
-      </c>
-      <c r="B99" s="9">
-        <v>0</v>
+      <c r="A99" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C99" t="s">
         <v>242</v>
@@ -6750,11 +6874,11 @@
       <c r="T99" s="9"/>
     </row>
     <row r="100" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="8">
-        <v>0</v>
-      </c>
-      <c r="B100" s="9">
-        <v>0</v>
+      <c r="A100" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="C100" t="s">
         <v>243</v>
@@ -6802,11 +6926,11 @@
       <c r="T100" s="9"/>
     </row>
     <row r="101" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="8">
-        <v>0</v>
-      </c>
-      <c r="B101" s="9">
-        <v>0</v>
+      <c r="A101" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="C101" t="s">
         <v>244</v>
@@ -6854,11 +6978,11 @@
       <c r="T101" s="9"/>
     </row>
     <row r="102" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="8">
-        <v>0</v>
-      </c>
-      <c r="B102" s="9">
-        <v>0</v>
+      <c r="A102" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C102" t="s">
         <v>245</v>
@@ -6906,11 +7030,11 @@
       <c r="T102" s="9"/>
     </row>
     <row r="103" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="8">
-        <v>0</v>
-      </c>
-      <c r="B103" s="9">
-        <v>0</v>
+      <c r="A103" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C103" t="s">
         <v>246</v>
@@ -6958,11 +7082,11 @@
       <c r="T103" s="9"/>
     </row>
     <row r="104" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="8">
-        <v>0</v>
-      </c>
-      <c r="B104" s="9">
-        <v>0</v>
+      <c r="A104" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="C104" t="s">
         <v>247</v>
@@ -7010,11 +7134,11 @@
       <c r="T104" s="9"/>
     </row>
     <row r="105" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="8">
-        <v>0</v>
-      </c>
-      <c r="B105" s="9">
-        <v>0</v>
+      <c r="A105" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C105" t="s">
         <v>248</v>
@@ -7062,11 +7186,11 @@
       <c r="T105" s="9"/>
     </row>
     <row r="106" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="8">
-        <v>0</v>
-      </c>
-      <c r="B106" s="9">
-        <v>0</v>
+      <c r="A106" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C106" t="s">
         <v>249</v>
@@ -7114,11 +7238,11 @@
       <c r="T106" s="9"/>
     </row>
     <row r="107" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="8">
-        <v>0</v>
-      </c>
-      <c r="B107" s="9">
-        <v>0</v>
+      <c r="A107" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C107" t="s">
         <v>250</v>
@@ -7166,11 +7290,11 @@
       <c r="T107" s="9"/>
     </row>
     <row r="108" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="8">
-        <v>0</v>
-      </c>
-      <c r="B108" s="9">
-        <v>0</v>
+      <c r="A108" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C108" t="s">
         <v>251</v>
@@ -7218,11 +7342,11 @@
       <c r="T108" s="9"/>
     </row>
     <row r="109" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="8">
-        <v>0</v>
-      </c>
-      <c r="B109" s="9">
-        <v>0</v>
+      <c r="A109" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C109" t="s">
         <v>252</v>
@@ -7270,11 +7394,11 @@
       <c r="T109" s="9"/>
     </row>
     <row r="110" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="8">
-        <v>0</v>
-      </c>
-      <c r="B110" s="9">
-        <v>0</v>
+      <c r="A110" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C110" t="s">
         <v>253</v>
@@ -7322,11 +7446,11 @@
       <c r="T110" s="9"/>
     </row>
     <row r="111" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="8">
-        <v>0</v>
-      </c>
-      <c r="B111" s="9">
-        <v>0</v>
+      <c r="A111" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C111" t="s">
         <v>254</v>
@@ -7374,11 +7498,11 @@
       <c r="T111" s="9"/>
     </row>
     <row r="112" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="8">
-        <v>0</v>
-      </c>
-      <c r="B112" s="9">
-        <v>0</v>
+      <c r="A112" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C112" t="s">
         <v>255</v>
@@ -7426,11 +7550,11 @@
       <c r="T112" s="9"/>
     </row>
     <row r="113" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="8">
-        <v>0</v>
-      </c>
-      <c r="B113" s="9">
-        <v>0</v>
+      <c r="A113" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C113" t="s">
         <v>256</v>
@@ -7478,11 +7602,11 @@
       <c r="T113" s="9"/>
     </row>
     <row r="114" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="8">
-        <v>0</v>
-      </c>
-      <c r="B114" s="9">
-        <v>0</v>
+      <c r="A114" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C114" t="s">
         <v>257</v>
@@ -7530,11 +7654,11 @@
       <c r="T114" s="9"/>
     </row>
     <row r="115" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="8">
-        <v>0</v>
-      </c>
-      <c r="B115" s="9">
-        <v>0</v>
+      <c r="A115" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C115" t="s">
         <v>258</v>
@@ -7582,11 +7706,11 @@
       <c r="T115" s="9"/>
     </row>
     <row r="116" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="8">
-        <v>0</v>
-      </c>
-      <c r="B116" s="9">
-        <v>0</v>
+      <c r="A116" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C116" t="s">
         <v>259</v>
@@ -7634,11 +7758,11 @@
       <c r="T116" s="9"/>
     </row>
     <row r="117" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="8">
-        <v>0</v>
-      </c>
-      <c r="B117" s="9">
-        <v>0</v>
+      <c r="A117" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C117" t="s">
         <v>260</v>
@@ -7686,11 +7810,11 @@
       <c r="T117" s="9"/>
     </row>
     <row r="118" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="8">
-        <v>0</v>
-      </c>
-      <c r="B118" s="9">
-        <v>0</v>
+      <c r="A118" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C118" t="s">
         <v>261</v>
@@ -7738,11 +7862,11 @@
       <c r="T118" s="9"/>
     </row>
     <row r="119" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="8">
-        <v>0</v>
-      </c>
-      <c r="B119" s="9">
-        <v>0</v>
+      <c r="A119" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C119" t="s">
         <v>262</v>
@@ -7790,11 +7914,11 @@
       <c r="T119" s="9"/>
     </row>
     <row r="120" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="8">
-        <v>0</v>
-      </c>
-      <c r="B120" s="9">
-        <v>0</v>
+      <c r="A120" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C120" t="s">
         <v>263</v>
@@ -7842,11 +7966,11 @@
       <c r="T120" s="9"/>
     </row>
     <row r="121" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="8">
-        <v>0</v>
-      </c>
-      <c r="B121" s="9">
-        <v>0</v>
+      <c r="A121" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C121" t="s">
         <v>264</v>
@@ -7894,11 +8018,11 @@
       <c r="T121" s="9"/>
     </row>
     <row r="122" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="8">
-        <v>0</v>
-      </c>
-      <c r="B122" s="9">
-        <v>0</v>
+      <c r="A122" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C122" t="s">
         <v>265</v>
@@ -7946,11 +8070,11 @@
       <c r="T122" s="9"/>
     </row>
     <row r="123" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="8">
-        <v>0</v>
-      </c>
-      <c r="B123" s="9">
-        <v>0</v>
+      <c r="A123" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C123" t="s">
         <v>266</v>
@@ -7998,11 +8122,11 @@
       <c r="T123" s="9"/>
     </row>
     <row r="124" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="8">
-        <v>0</v>
-      </c>
-      <c r="B124" s="9">
-        <v>0</v>
+      <c r="A124" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>347</v>
       </c>
       <c r="C124" t="s">
         <v>267</v>
@@ -8050,11 +8174,11 @@
       <c r="T124" s="9"/>
     </row>
     <row r="125" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="8">
-        <v>0</v>
-      </c>
-      <c r="B125" s="9">
-        <v>0</v>
+      <c r="A125" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>347</v>
       </c>
       <c r="C125" t="s">
         <v>268</v>
@@ -8102,11 +8226,11 @@
       <c r="T125" s="9"/>
     </row>
     <row r="126" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="8">
-        <v>0</v>
-      </c>
-      <c r="B126" s="9">
-        <v>0</v>
+      <c r="A126" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C126" t="s">
         <v>269</v>
@@ -8154,11 +8278,11 @@
       <c r="T126" s="9"/>
     </row>
     <row r="127" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="8">
-        <v>0</v>
-      </c>
-      <c r="B127" s="9">
-        <v>0</v>
+      <c r="A127" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C127" t="s">
         <v>270</v>
@@ -8206,11 +8330,11 @@
       <c r="T127" s="9"/>
     </row>
     <row r="128" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="8">
-        <v>0</v>
-      </c>
-      <c r="B128" s="9">
-        <v>0</v>
+      <c r="A128" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C128" t="s">
         <v>271</v>
@@ -8258,11 +8382,11 @@
       <c r="T128" s="9"/>
     </row>
     <row r="129" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="8">
-        <v>0</v>
-      </c>
-      <c r="B129" s="9">
-        <v>0</v>
+      <c r="A129" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C129" t="s">
         <v>272</v>
@@ -8310,11 +8434,11 @@
       <c r="T129" s="9"/>
     </row>
     <row r="130" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="8">
-        <v>0</v>
-      </c>
-      <c r="B130" s="9">
-        <v>0</v>
+      <c r="A130" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C130" t="s">
         <v>273</v>
@@ -8362,11 +8486,11 @@
       <c r="T130" s="9"/>
     </row>
     <row r="131" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="8">
-        <v>0</v>
-      </c>
-      <c r="B131" s="9">
-        <v>0</v>
+      <c r="A131" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C131" t="s">
         <v>274</v>
@@ -8414,11 +8538,11 @@
       <c r="T131" s="9"/>
     </row>
     <row r="132" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="8">
-        <v>0</v>
-      </c>
-      <c r="B132" s="9">
-        <v>0</v>
+      <c r="A132" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C132" t="s">
         <v>275</v>
@@ -8466,11 +8590,11 @@
       <c r="T132" s="9"/>
     </row>
     <row r="133" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="8">
-        <v>0</v>
-      </c>
-      <c r="B133" s="9">
-        <v>0</v>
+      <c r="A133" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C133" t="s">
         <v>276</v>
@@ -8518,11 +8642,11 @@
       <c r="T133" s="9"/>
     </row>
     <row r="134" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="8">
-        <v>0</v>
-      </c>
-      <c r="B134" s="9">
-        <v>0</v>
+      <c r="A134" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C134" t="s">
         <v>277</v>
@@ -8570,11 +8694,11 @@
       <c r="T134" s="9"/>
     </row>
     <row r="135" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="8">
-        <v>0</v>
-      </c>
-      <c r="B135" s="9">
-        <v>0</v>
+      <c r="A135" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C135" t="s">
         <v>278</v>
@@ -8622,11 +8746,11 @@
       <c r="T135" s="9"/>
     </row>
     <row r="136" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="8">
-        <v>0</v>
-      </c>
-      <c r="B136" s="9">
-        <v>0</v>
+      <c r="A136" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C136" t="s">
         <v>279</v>
@@ -8674,11 +8798,11 @@
       <c r="T136" s="9"/>
     </row>
     <row r="137" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="8">
-        <v>0</v>
-      </c>
-      <c r="B137" s="9">
-        <v>0</v>
+      <c r="A137" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C137" t="s">
         <v>280</v>
@@ -8726,11 +8850,11 @@
       <c r="T137" s="9"/>
     </row>
     <row r="138" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="8">
-        <v>0</v>
-      </c>
-      <c r="B138" s="9">
-        <v>0</v>
+      <c r="A138" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C138" t="s">
         <v>281</v>
@@ -8778,11 +8902,11 @@
       <c r="T138" s="9"/>
     </row>
     <row r="139" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="8">
-        <v>0</v>
-      </c>
-      <c r="B139" s="9">
-        <v>0</v>
+      <c r="A139" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C139" t="s">
         <v>282</v>
@@ -8830,11 +8954,11 @@
       <c r="T139" s="9"/>
     </row>
     <row r="140" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="8">
-        <v>0</v>
-      </c>
-      <c r="B140" s="9">
-        <v>0</v>
+      <c r="A140" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>348</v>
       </c>
       <c r="C140" t="s">
         <v>283</v>
@@ -8882,11 +9006,11 @@
       <c r="T140" s="9"/>
     </row>
     <row r="141" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="8">
-        <v>0</v>
-      </c>
-      <c r="B141" s="9">
-        <v>0</v>
+      <c r="A141" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>349</v>
       </c>
       <c r="C141" t="s">
         <v>284</v>
@@ -8934,11 +9058,11 @@
       <c r="T141" s="9"/>
     </row>
     <row r="142" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="8">
-        <v>0</v>
-      </c>
-      <c r="B142" s="9">
-        <v>0</v>
+      <c r="A142" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>349</v>
       </c>
       <c r="C142" t="s">
         <v>285</v>
@@ -8986,11 +9110,11 @@
       <c r="T142" s="9"/>
     </row>
     <row r="143" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="8">
-        <v>0</v>
-      </c>
-      <c r="B143" s="9">
-        <v>0</v>
+      <c r="A143" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="C143" t="s">
         <v>286</v>
@@ -9038,11 +9162,11 @@
       <c r="T143" s="9"/>
     </row>
     <row r="144" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="8">
-        <v>0</v>
-      </c>
-      <c r="B144" s="9">
-        <v>0</v>
+      <c r="A144" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="C144" t="s">
         <v>287</v>
@@ -9090,11 +9214,11 @@
       <c r="T144" s="9"/>
     </row>
     <row r="145" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="8">
-        <v>0</v>
-      </c>
-      <c r="B145" s="9">
-        <v>0</v>
+      <c r="A145" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="C145" t="s">
         <v>288</v>
@@ -9142,11 +9266,11 @@
       <c r="T145" s="9"/>
     </row>
     <row r="146" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="8">
-        <v>0</v>
-      </c>
-      <c r="B146" s="9">
-        <v>0</v>
+      <c r="A146" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="C146" t="s">
         <v>289</v>
@@ -9194,11 +9318,11 @@
       <c r="T146" s="9"/>
     </row>
     <row r="147" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="8">
-        <v>0</v>
-      </c>
-      <c r="B147" s="9">
-        <v>0</v>
+      <c r="A147" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>346</v>
       </c>
       <c r="C147" t="s">
         <v>290</v>
@@ -9246,11 +9370,11 @@
       <c r="T147" s="9"/>
     </row>
     <row r="148" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="8">
-        <v>0</v>
-      </c>
-      <c r="B148" s="9">
-        <v>0</v>
+      <c r="A148" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>349</v>
       </c>
       <c r="C148" t="s">
         <v>291</v>
@@ -9298,11 +9422,11 @@
       <c r="T148" s="9"/>
     </row>
     <row r="149" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="8">
-        <v>0</v>
-      </c>
-      <c r="B149" s="9">
-        <v>0</v>
+      <c r="A149" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>350</v>
       </c>
       <c r="C149" t="s">
         <v>292</v>
@@ -9350,11 +9474,11 @@
       <c r="T149" s="9"/>
     </row>
     <row r="150" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="8">
-        <v>0</v>
-      </c>
-      <c r="B150" s="9">
-        <v>0</v>
+      <c r="A150" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>352</v>
       </c>
       <c r="C150" t="s">
         <v>293</v>
@@ -9402,11 +9526,11 @@
       <c r="T150" s="9"/>
     </row>
     <row r="151" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="8">
-        <v>0</v>
-      </c>
-      <c r="B151" s="9">
-        <v>0</v>
+      <c r="A151" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C151" t="s">
         <v>294</v>
@@ -9454,11 +9578,11 @@
       <c r="T151" s="9"/>
     </row>
     <row r="152" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="8">
-        <v>0</v>
-      </c>
-      <c r="B152" s="9">
-        <v>0</v>
+      <c r="A152" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C152" t="s">
         <v>295</v>
@@ -9506,11 +9630,11 @@
       <c r="T152" s="9"/>
     </row>
     <row r="153" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="8">
-        <v>0</v>
-      </c>
-      <c r="B153" s="9">
-        <v>0</v>
+      <c r="A153" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C153" t="s">
         <v>296</v>
@@ -9558,11 +9682,11 @@
       <c r="T153" s="9"/>
     </row>
     <row r="154" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="8">
-        <v>0</v>
-      </c>
-      <c r="B154" s="9">
-        <v>0</v>
+      <c r="A154" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>355</v>
       </c>
       <c r="C154" t="s">
         <v>297</v>
@@ -9610,11 +9734,11 @@
       <c r="T154" s="9"/>
     </row>
     <row r="155" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="8">
-        <v>0</v>
-      </c>
-      <c r="B155" s="9">
-        <v>0</v>
+      <c r="A155" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>355</v>
       </c>
       <c r="C155" t="s">
         <v>298</v>
@@ -9662,11 +9786,11 @@
       <c r="T155" s="9"/>
     </row>
     <row r="156" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="8">
-        <v>0</v>
-      </c>
-      <c r="B156" s="9">
-        <v>0</v>
+      <c r="A156" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>355</v>
       </c>
       <c r="C156" t="s">
         <v>299</v>
@@ -9714,11 +9838,11 @@
       <c r="T156" s="9"/>
     </row>
     <row r="157" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="8">
-        <v>0</v>
-      </c>
-      <c r="B157" s="9">
-        <v>0</v>
+      <c r="A157" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C157" t="s">
         <v>300</v>
@@ -9766,11 +9890,11 @@
       <c r="T157" s="9"/>
     </row>
     <row r="158" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="8">
-        <v>0</v>
-      </c>
-      <c r="B158" s="9">
-        <v>0</v>
+      <c r="A158" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>357</v>
       </c>
       <c r="C158" t="s">
         <v>301</v>
@@ -9818,11 +9942,11 @@
       <c r="T158" s="9"/>
     </row>
     <row r="159" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="8">
-        <v>0</v>
-      </c>
-      <c r="B159" s="9">
-        <v>0</v>
+      <c r="A159" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>357</v>
       </c>
       <c r="C159" t="s">
         <v>302</v>
@@ -9870,11 +9994,11 @@
       <c r="T159" s="9"/>
     </row>
     <row r="160" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="8">
-        <v>0</v>
-      </c>
-      <c r="B160" s="9">
-        <v>0</v>
+      <c r="A160" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>357</v>
       </c>
       <c r="C160" t="s">
         <v>303</v>
@@ -9922,11 +10046,11 @@
       <c r="T160" s="9"/>
     </row>
     <row r="161" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="8">
-        <v>0</v>
-      </c>
-      <c r="B161" s="9">
-        <v>0</v>
+      <c r="A161" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>358</v>
       </c>
       <c r="C161" t="s">
         <v>304</v>
@@ -9974,11 +10098,11 @@
       <c r="T161" s="9"/>
     </row>
     <row r="162" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="8">
-        <v>0</v>
-      </c>
-      <c r="B162" s="9">
-        <v>0</v>
+      <c r="A162" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>358</v>
       </c>
       <c r="C162" t="s">
         <v>305</v>
@@ -10026,11 +10150,11 @@
       <c r="T162" s="9"/>
     </row>
     <row r="163" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="8">
-        <v>0</v>
-      </c>
-      <c r="B163" s="9">
-        <v>0</v>
+      <c r="A163" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B163" s="9" t="s">
+        <v>359</v>
       </c>
       <c r="C163" t="s">
         <v>306</v>
@@ -10078,11 +10202,11 @@
       <c r="T163" s="9"/>
     </row>
     <row r="164" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="8">
-        <v>0</v>
-      </c>
-      <c r="B164" s="9">
-        <v>0</v>
+      <c r="A164" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C164" t="s">
         <v>307</v>
@@ -10130,11 +10254,11 @@
       <c r="T164" s="9"/>
     </row>
     <row r="165" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="8">
-        <v>0</v>
-      </c>
-      <c r="B165" s="9">
-        <v>0</v>
+      <c r="A165" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B165" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C165" t="s">
         <v>308</v>
@@ -10182,11 +10306,11 @@
       <c r="T165" s="9"/>
     </row>
     <row r="166" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="8">
-        <v>0</v>
-      </c>
-      <c r="B166" s="9">
-        <v>0</v>
+      <c r="A166" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B166" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C166" t="s">
         <v>309</v>
@@ -10234,11 +10358,11 @@
       <c r="T166" s="9"/>
     </row>
     <row r="167" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="8">
-        <v>0</v>
-      </c>
-      <c r="B167" s="9">
-        <v>0</v>
+      <c r="A167" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C167" t="s">
         <v>310</v>
@@ -10286,11 +10410,11 @@
       <c r="T167" s="9"/>
     </row>
     <row r="168" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="8">
-        <v>0</v>
-      </c>
-      <c r="B168" s="9">
-        <v>0</v>
+      <c r="A168" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C168" t="s">
         <v>311</v>
@@ -10338,11 +10462,11 @@
       <c r="T168" s="9"/>
     </row>
     <row r="169" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="8">
-        <v>0</v>
-      </c>
-      <c r="B169" s="9">
-        <v>0</v>
+      <c r="A169" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B169" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C169" t="s">
         <v>312</v>
@@ -10390,11 +10514,11 @@
       <c r="T169" s="9"/>
     </row>
     <row r="170" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="8">
-        <v>0</v>
-      </c>
-      <c r="B170" s="9">
-        <v>0</v>
+      <c r="A170" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C170" t="s">
         <v>313</v>
@@ -10442,11 +10566,11 @@
       <c r="T170" s="9"/>
     </row>
     <row r="171" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="8">
-        <v>0</v>
-      </c>
-      <c r="B171" s="9">
-        <v>0</v>
+      <c r="A171" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B171" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C171" t="s">
         <v>314</v>
@@ -10494,11 +10618,11 @@
       <c r="T171" s="9"/>
     </row>
     <row r="172" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="8">
-        <v>0</v>
-      </c>
-      <c r="B172" s="9">
-        <v>0</v>
+      <c r="A172" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B172" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C172" t="s">
         <v>315</v>
@@ -10546,11 +10670,11 @@
       <c r="T172" s="9"/>
     </row>
     <row r="173" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="8">
-        <v>0</v>
-      </c>
-      <c r="B173" s="9">
-        <v>0</v>
+      <c r="A173" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B173" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C173" t="s">
         <v>316</v>
@@ -10598,11 +10722,11 @@
       <c r="T173" s="9"/>
     </row>
     <row r="174" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="8">
-        <v>0</v>
-      </c>
-      <c r="B174" s="9">
-        <v>0</v>
+      <c r="A174" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B174" s="9" t="s">
+        <v>360</v>
       </c>
       <c r="C174" t="s">
         <v>317</v>
@@ -10650,11 +10774,11 @@
       <c r="T174" s="9"/>
     </row>
     <row r="175" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="8">
-        <v>0</v>
-      </c>
-      <c r="B175" s="9">
-        <v>0</v>
+      <c r="A175" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B175" s="9" t="s">
+        <v>360</v>
       </c>
       <c r="C175" t="s">
         <v>318</v>
@@ -10702,11 +10826,11 @@
       <c r="T175" s="9"/>
     </row>
     <row r="176" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="8">
-        <v>0</v>
-      </c>
-      <c r="B176" s="9">
-        <v>0</v>
+      <c r="A176" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B176" s="9" t="s">
+        <v>360</v>
       </c>
       <c r="C176" t="s">
         <v>319</v>
@@ -10754,11 +10878,11 @@
       <c r="T176" s="9"/>
     </row>
     <row r="177" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="8">
-        <v>0</v>
-      </c>
-      <c r="B177" s="9">
-        <v>0</v>
+      <c r="A177" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B177" s="9" t="s">
+        <v>361</v>
       </c>
       <c r="C177" t="s">
         <v>320</v>
@@ -10806,11 +10930,11 @@
       <c r="T177" s="9"/>
     </row>
     <row r="178" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="8">
-        <v>0</v>
-      </c>
-      <c r="B178" s="9">
-        <v>0</v>
+      <c r="A178" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B178" s="9" t="s">
+        <v>361</v>
       </c>
       <c r="C178" t="s">
         <v>321</v>
@@ -10858,11 +10982,11 @@
       <c r="T178" s="9"/>
     </row>
     <row r="179" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="8">
-        <v>0</v>
-      </c>
-      <c r="B179" s="9">
-        <v>0</v>
+      <c r="A179" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B179" s="9" t="s">
+        <v>361</v>
       </c>
       <c r="C179" t="s">
         <v>322</v>
@@ -10910,11 +11034,11 @@
       <c r="T179" s="9"/>
     </row>
     <row r="180" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="8">
-        <v>0</v>
-      </c>
-      <c r="B180" s="9">
-        <v>0</v>
+      <c r="A180" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B180" s="9" t="s">
+        <v>361</v>
       </c>
       <c r="C180" t="s">
         <v>323</v>
@@ -10962,11 +11086,11 @@
       <c r="T180" s="9"/>
     </row>
     <row r="181" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="8">
-        <v>0</v>
-      </c>
-      <c r="B181" s="9">
-        <v>0</v>
+      <c r="A181" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B181" s="9" t="s">
+        <v>361</v>
       </c>
       <c r="C181" t="s">
         <v>324</v>
@@ -11014,11 +11138,11 @@
       <c r="T181" s="9"/>
     </row>
     <row r="182" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="8">
-        <v>0</v>
-      </c>
-      <c r="B182" s="9">
-        <v>0</v>
+      <c r="A182" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B182" s="9" t="s">
+        <v>361</v>
       </c>
       <c r="C182" t="s">
         <v>325</v>
@@ -11066,11 +11190,11 @@
       <c r="T182" s="9"/>
     </row>
     <row r="183" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="8">
-        <v>0</v>
-      </c>
-      <c r="B183" s="9">
-        <v>0</v>
+      <c r="A183" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B183" s="9" t="s">
+        <v>361</v>
       </c>
       <c r="C183" t="s">
         <v>326</v>
@@ -11118,11 +11242,11 @@
       <c r="T183" s="9"/>
     </row>
     <row r="184" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="8">
-        <v>0</v>
-      </c>
-      <c r="B184" s="9">
-        <v>0</v>
+      <c r="A184" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B184" s="9" t="s">
+        <v>362</v>
       </c>
       <c r="C184" t="s">
         <v>327</v>
@@ -11170,11 +11294,11 @@
       <c r="T184" s="9"/>
     </row>
     <row r="185" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="8">
-        <v>0</v>
-      </c>
-      <c r="B185" s="9">
-        <v>0</v>
+      <c r="A185" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B185" s="9" t="s">
+        <v>362</v>
       </c>
       <c r="C185" t="s">
         <v>328</v>
@@ -11222,11 +11346,11 @@
       <c r="T185" s="9"/>
     </row>
     <row r="186" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="8">
-        <v>0</v>
-      </c>
-      <c r="B186" s="9">
-        <v>0</v>
+      <c r="A186" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B186" s="9" t="s">
+        <v>362</v>
       </c>
       <c r="C186" t="s">
         <v>329</v>
@@ -11274,11 +11398,11 @@
       <c r="T186" s="9"/>
     </row>
     <row r="187" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="8">
-        <v>0</v>
-      </c>
-      <c r="B187" s="9">
-        <v>0</v>
+      <c r="A187" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B187" s="9" t="s">
+        <v>362</v>
       </c>
       <c r="C187" t="s">
         <v>330</v>
@@ -11326,11 +11450,11 @@
       <c r="T187" s="9"/>
     </row>
     <row r="188" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="8">
-        <v>0</v>
-      </c>
-      <c r="B188" s="9">
-        <v>0</v>
+      <c r="A188" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B188" s="9" t="s">
+        <v>362</v>
       </c>
       <c r="C188" t="s">
         <v>331</v>
@@ -11378,11 +11502,11 @@
       <c r="T188" s="9"/>
     </row>
     <row r="189" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="8">
-        <v>0</v>
-      </c>
-      <c r="B189" s="9">
-        <v>0</v>
+      <c r="A189" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B189" s="9" t="s">
+        <v>363</v>
       </c>
       <c r="C189" t="s">
         <v>332</v>
@@ -11430,11 +11554,11 @@
       <c r="T189" s="9"/>
     </row>
     <row r="190" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="8">
-        <v>0</v>
-      </c>
-      <c r="B190" s="9">
-        <v>0</v>
+      <c r="A190" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B190" s="9" t="s">
+        <v>363</v>
       </c>
       <c r="C190" t="s">
         <v>333</v>
@@ -11482,11 +11606,11 @@
       <c r="T190" s="9"/>
     </row>
     <row r="191" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="8">
-        <v>0</v>
-      </c>
-      <c r="B191" s="9">
-        <v>0</v>
+      <c r="A191" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B191" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="C191" t="s">
         <v>334</v>
@@ -11534,11 +11658,11 @@
       <c r="T191" s="9"/>
     </row>
     <row r="192" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="8">
-        <v>0</v>
-      </c>
-      <c r="B192" s="9">
-        <v>0</v>
+      <c r="A192" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B192" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="C192" t="s">
         <v>335</v>
@@ -11586,11 +11710,11 @@
       <c r="T192" s="9"/>
     </row>
     <row r="193" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="8">
-        <v>0</v>
-      </c>
-      <c r="B193" s="9">
-        <v>0</v>
+      <c r="A193" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B193" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="C193" t="s">
         <v>336</v>
@@ -11638,11 +11762,11 @@
       <c r="T193" s="9"/>
     </row>
     <row r="194" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="8">
-        <v>0</v>
-      </c>
-      <c r="B194" s="9">
-        <v>0</v>
+      <c r="A194" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B194" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="C194" t="s">
         <v>337</v>
@@ -11690,11 +11814,11 @@
       <c r="T194" s="9"/>
     </row>
     <row r="195" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="8">
-        <v>0</v>
-      </c>
-      <c r="B195" s="9">
-        <v>0</v>
+      <c r="A195" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B195" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="C195" t="s">
         <v>338</v>
@@ -11742,11 +11866,11 @@
       <c r="T195" s="9"/>
     </row>
     <row r="196" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="8">
-        <v>0</v>
-      </c>
-      <c r="B196" s="9">
-        <v>0</v>
+      <c r="A196" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B196" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="C196" t="s">
         <v>339</v>
@@ -11794,11 +11918,11 @@
       <c r="T196" s="9"/>
     </row>
     <row r="197" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="8">
-        <v>0</v>
-      </c>
-      <c r="B197" s="9">
-        <v>0</v>
+      <c r="A197" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B197" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C197" t="s">
         <v>340</v>
@@ -11846,11 +11970,11 @@
       <c r="T197" s="9"/>
     </row>
     <row r="198" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="8">
-        <v>0</v>
-      </c>
-      <c r="B198" s="9">
-        <v>0</v>
+      <c r="A198" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B198" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C198" t="s">
         <v>341</v>
@@ -11898,11 +12022,11 @@
       <c r="T198" s="9"/>
     </row>
     <row r="199" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="8">
-        <v>0</v>
-      </c>
-      <c r="B199" s="9">
-        <v>0</v>
+      <c r="A199" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B199" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C199" t="s">
         <v>342</v>
@@ -11950,11 +12074,11 @@
       <c r="T199" s="9"/>
     </row>
     <row r="200" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="8">
-        <v>0</v>
-      </c>
-      <c r="B200" s="9">
-        <v>0</v>
+      <c r="A200" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B200" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="C200" t="s">
         <v>343</v>
@@ -12002,11 +12126,11 @@
       <c r="T200" s="9"/>
     </row>
     <row r="201" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="10">
-        <v>0</v>
-      </c>
-      <c r="B201" s="11">
-        <v>0</v>
+      <c r="A201" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="B201" s="11" t="s">
+        <v>354</v>
       </c>
       <c r="C201" s="17" t="s">
         <v>344</v>

</xml_diff>

<commit_message>
aggreg update for liquid fuels
</commit_message>
<xml_diff>
--- a/data/aggregation/IMACLIM_format.xlsx
+++ b/data/aggregation/IMACLIM_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mpotfer\Stage\MatMat-Trade\data\aggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B92BF6-2BC1-46EC-995D-878A973DE65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1672FD63-8F7F-4F84-8D1D-40EAA7BD1A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1650,8 +1650,8 @@
   <dimension ref="A1:T202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J78" sqref="J78"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5440,13 +5440,13 @@
         <v>0</v>
       </c>
       <c r="K73" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L73" s="16">
         <v>0</v>
       </c>
       <c r="M73" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N73" s="16">
         <v>0</v>
@@ -5492,13 +5492,13 @@
         <v>0</v>
       </c>
       <c r="K74" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L74" s="16">
         <v>0</v>
       </c>
       <c r="M74" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N74" s="16">
         <v>0</v>

</xml_diff>

<commit_message>
aggreg up to date
</commit_message>
<xml_diff>
--- a/data/aggregation/IMACLIM_format.xlsx
+++ b/data/aggregation/IMACLIM_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mpotfer\Stage\MatMat-Trade\data\aggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01AF5E5-0F35-4594-93D5-0AE6DDB2245B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00AC6BD-7400-484B-92D5-8978D08570B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1650,8 +1650,8 @@
   <dimension ref="A1:T202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C164" sqref="C164"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G172" sqref="G172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6165,7 +6165,7 @@
         <v>0</v>
       </c>
       <c r="J87" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K87" s="16">
         <v>0</v>
@@ -6177,7 +6177,7 @@
         <v>0</v>
       </c>
       <c r="N87" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O87" s="16">
         <v>0</v>
@@ -6217,7 +6217,7 @@
         <v>0</v>
       </c>
       <c r="J88" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K88" s="16">
         <v>0</v>
@@ -6229,7 +6229,7 @@
         <v>0</v>
       </c>
       <c r="N88" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O88" s="16">
         <v>0</v>
@@ -7985,7 +7985,7 @@
         <v>0</v>
       </c>
       <c r="J122" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K122" s="16">
         <v>0</v>
@@ -7997,7 +7997,7 @@
         <v>0</v>
       </c>
       <c r="N122" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O122" s="16">
         <v>0</v>
@@ -8297,7 +8297,7 @@
         <v>0</v>
       </c>
       <c r="J128" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K128" s="16">
         <v>0</v>
@@ -8309,7 +8309,7 @@
         <v>0</v>
       </c>
       <c r="N128" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O128" s="16">
         <v>0</v>
@@ -8967,7 +8967,7 @@
         <v>0</v>
       </c>
       <c r="H141" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I141" s="16">
         <v>0</v>
@@ -8985,7 +8985,7 @@
         <v>0</v>
       </c>
       <c r="N141" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O141" s="16">
         <v>0</v>
@@ -9019,7 +9019,7 @@
         <v>0</v>
       </c>
       <c r="H142" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I142" s="16">
         <v>0</v>
@@ -9037,7 +9037,7 @@
         <v>0</v>
       </c>
       <c r="N142" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O142" s="16">
         <v>0</v>
@@ -9334,7 +9334,7 @@
         <v>0</v>
       </c>
       <c r="I148" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J148" s="16">
         <v>0</v>
@@ -9349,7 +9349,7 @@
         <v>0</v>
       </c>
       <c r="N148" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O148" s="16">
         <v>0</v>
@@ -9386,7 +9386,7 @@
         <v>0</v>
       </c>
       <c r="I149" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J149" s="16">
         <v>0</v>
@@ -9401,7 +9401,7 @@
         <v>0</v>
       </c>
       <c r="N149" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O149" s="16">
         <v>0</v>
@@ -10839,13 +10839,13 @@
         <v>0</v>
       </c>
       <c r="H177" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I177" s="16">
         <v>0</v>
       </c>
       <c r="J177" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K177" s="16">
         <v>0</v>
@@ -10891,13 +10891,13 @@
         <v>0</v>
       </c>
       <c r="H178" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I178" s="16">
         <v>0</v>
       </c>
       <c r="J178" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K178" s="16">
         <v>0</v>
@@ -10943,13 +10943,13 @@
         <v>0</v>
       </c>
       <c r="H179" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I179" s="16">
         <v>0</v>
       </c>
       <c r="J179" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K179" s="16">
         <v>0</v>
@@ -10995,13 +10995,13 @@
         <v>0</v>
       </c>
       <c r="H180" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I180" s="16">
         <v>0</v>
       </c>
       <c r="J180" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K180" s="16">
         <v>0</v>
@@ -11047,13 +11047,13 @@
         <v>0</v>
       </c>
       <c r="H181" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I181" s="16">
         <v>0</v>
       </c>
       <c r="J181" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K181" s="16">
         <v>0</v>
@@ -11099,13 +11099,13 @@
         <v>0</v>
       </c>
       <c r="H182" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I182" s="16">
         <v>0</v>
       </c>
       <c r="J182" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K182" s="16">
         <v>0</v>
@@ -11151,13 +11151,13 @@
         <v>0</v>
       </c>
       <c r="H183" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I183" s="16">
         <v>0</v>
       </c>
       <c r="J183" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K183" s="16">
         <v>0</v>

</xml_diff>